<commit_message>
activity_relation_data_stats: update stats after adjusting activity relation generation
</commit_message>
<xml_diff>
--- a/data/paper_stats/activity_relation/branch_lengths.xlsx
+++ b/data/paper_stats/activity_relation/branch_lengths.xlsx
@@ -1403,7 +1403,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -1493,7 +1493,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -1813,7 +1813,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
@@ -2069,7 +2069,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.60126582278481</v>
+        <v>2.537974683544304</v>
       </c>
     </row>
     <row r="4">
@@ -2079,7 +2079,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3.367018514073111</v>
+        <v>3.364551201745027</v>
       </c>
     </row>
     <row r="5">
@@ -2119,7 +2119,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">

</xml_diff>